<commit_message>
Updated BACIPS for PVR with 2020 as impact and 10 year dataset.
</commit_message>
<xml_diff>
--- a/BACIPS_UniqueSites_Sep22.xlsx
+++ b/BACIPS_UniqueSites_Sep22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssaplayer/Desktop/AP-VRG-PVR-RefugiaAR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2BEED58E-74A3-7744-935C-16973C4D2D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B85377B3-68B9-1C43-8481-5A0F4CA29E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="760" windowWidth="19180" windowHeight="17400" xr2:uid="{CC2E8A42-1982-EF41-9685-F571566A1875}"/>
+    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="17360" xr2:uid="{CC2E8A42-1982-EF41-9685-F571566A1875}"/>
   </bookViews>
   <sheets>
     <sheet name="PVRControlImpactSites_Unique_Se" sheetId="1" r:id="rId1"/>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF12B1FA-8A2E-6B4A-A9CB-FAA64EBB40CE}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>